<commit_message>
test - Commented GitLatch Commit @ 2024-6-25-10-38-14-695
</commit_message>
<xml_diff>
--- a/Test Table.xlsx
+++ b/Test Table.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27813"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\appsure\Desktop\Testing Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04CB44CF-F477-44F2-9B15-B36AF382A9E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -38,38 +50,38 @@
     <t>test3</t>
   </si>
   <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>gadf</t>
+  </si>
+  <si>
+    <t>daf</t>
+  </si>
+  <si>
+    <t>fga</t>
+  </si>
+  <si>
+    <t>adg</t>
+  </si>
+  <si>
+    <t>dfga</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>afd</t>
+  </si>
+  <si>
     <t>gf</t>
   </si>
-  <si>
-    <t>dfga</t>
-  </si>
-  <si>
-    <t>afd</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>daf</t>
-  </si>
-  <si>
-    <t>gadf</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>fga</t>
-  </si>
-  <si>
-    <t>adg</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +130,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="E3:H13" totalsRowShown="0">
-  <autoFilter ref="E3:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="E3:H13" totalsRowShown="0">
+  <autoFilter ref="E3:H13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="test"/>
-    <tableColumn id="2" name="test2"/>
-    <tableColumn id="3" name="test22"/>
-    <tableColumn id="4" name="test3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="test"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="test2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="test22"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="test3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -396,6 +408,9 @@
   <wetp:taskpane dockstate="right" visibility="0" width="976" row="1">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="1" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -408,23 +423,47 @@
     <we:binding id="VisualizationTable" type="table" appref="{A8195AAD-DC9F-4A1C-B5A9-F69834264723}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+  </we:extLst>
 </we:webextension>
 </file>
 
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{34DAC5CE-9CD7-487C-8DBB-CB6751B09242}">
+  <we:reference id="9872a169-49e5-4c4b-b9e3-3ebf124a5933" version="1.0.0.1" store="developer" storeType="uploadfiledevcatalog"/>
+  <we:alternateReferences>
+    <we:reference id="9872a169-49e5-4c4b-b9e3-3ebf124a5933Office.AutoShowTaskpaneWithDocument" version="1.0.0.1" store="omex" storeType="omex"/>
+  </we:alternateReferences>
+  <we:properties>
+    <we:property name="Office.AutoShowTaskpaneWithDocument" value="true"/>
+  </we:properties>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="E3:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="5" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:11">
       <c r="E3" t="s">
         <v>0</v>
       </c>
@@ -437,10 +476,13 @@
       <c r="H3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="4" spans="5:11">
       <c r="E4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>9</v>
@@ -452,9 +494,9 @@
         <v>789</v>
       </c>
     </row>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:11">
       <c r="E5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>8</v>
@@ -466,9 +508,9 @@
         <v>798</v>
       </c>
     </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:11">
       <c r="E6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F6">
         <v>7</v>
@@ -480,9 +522,9 @@
         <v>789</v>
       </c>
     </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:11">
       <c r="E7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -494,9 +536,9 @@
         <v>789</v>
       </c>
     </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:11">
       <c r="E8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -505,9 +547,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:11">
       <c r="E9" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -519,9 +561,9 @@
         <v>789</v>
       </c>
     </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:11">
       <c r="E10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>3</v>
@@ -533,9 +575,9 @@
         <v>456</v>
       </c>
     </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:11">
       <c r="E11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -547,9 +589,9 @@
         <v>879</v>
       </c>
     </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:11">
       <c r="E12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -561,9 +603,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:11">
       <c r="E13" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F13">
         <v>0</v>

</xml_diff>

<commit_message>
Test123 - Commented GitLatch Commit @ 2024-6-25-16-56-17-14
</commit_message>
<xml_diff>
--- a/Test Table.xlsx
+++ b/Test Table.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27813"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10609"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\appsure\Desktop\Testing Docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73FC2D33-A32E-4C00-A7C9-98D2921695F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{84E8E7B6-93B4-AC4F-A130-3D6DE145B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -458,12 +453,12 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:11">
+    <row r="3" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>0</v>
       </c>
@@ -480,7 +475,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="4" spans="5:11">
+    <row r="4" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -494,7 +489,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="5" spans="5:11">
+    <row r="5" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>5</v>
       </c>
@@ -508,7 +503,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="6" spans="5:11">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>6</v>
       </c>
@@ -522,7 +517,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="7" spans="5:11">
+    <row r="7" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>7</v>
       </c>
@@ -536,7 +531,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="8" spans="5:11">
+    <row r="8" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>8</v>
       </c>
@@ -547,7 +542,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="5:11">
+    <row r="9" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>9</v>
       </c>
@@ -561,7 +556,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="10" spans="5:11">
+    <row r="10" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>10</v>
       </c>
@@ -575,7 +570,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="11" spans="5:11">
+    <row r="11" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>11</v>
       </c>
@@ -589,7 +584,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="12" spans="5:11">
+    <row r="12" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>9</v>
       </c>
@@ -603,7 +598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="5:11">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>12</v>
       </c>

</xml_diff>